<commit_message>
Add problem file 15 and 16
</commit_message>
<xml_diff>
--- a/problem_file_suite/problem_files.xlsx
+++ b/problem_file_suite/problem_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickit/Desktop/INT-Coursework-2021/problem_file_suite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B912E7E8-D314-1647-A6E7-B298E612C98F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AA6795-1806-1041-B70F-8C982D27B239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="4080" windowWidth="14380" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5360" yWindow="3340" windowWidth="18340" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,7 +436,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D13" si="0">B2*C2</f>
+        <f t="shared" ref="D2:D17" si="0">B2*C2</f>
         <v>36</v>
       </c>
       <c r="E2">
@@ -693,9 +693,105 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>510</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>493</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the map for problem 12-16
</commit_message>
<xml_diff>
--- a/problem_file_suite/problem_files.xlsx
+++ b/problem_file_suite/problem_files.xlsx
@@ -8,13 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickit/Desktop/INT-Coursework-2021/problem_file_suite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AA6795-1806-1041-B70F-8C982D27B239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163821C8-CF9C-0C46-B8EC-08BAEA80B32A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5360" yWindow="3340" windowWidth="18340" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$G$2:$G$17</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$H$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$2:$H$17</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$G$2:$G$17</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$H$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$H$2:$H$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -392,7 +402,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,6 +719,9 @@
       <c r="G13">
         <v>212</v>
       </c>
+      <c r="H13">
+        <v>-1</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -730,6 +743,9 @@
       <c r="G14">
         <v>233</v>
       </c>
+      <c r="H14">
+        <v>-1</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -751,6 +767,9 @@
       <c r="G15">
         <v>282</v>
       </c>
+      <c r="H15">
+        <v>-1</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -772,8 +791,11 @@
       <c r="G16">
         <v>335</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -791,6 +813,9 @@
         <v>1</v>
       </c>
       <c r="G17">
+        <v>429</v>
+      </c>
+      <c r="H17">
         <v>429</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add execution results with pliers to the Excel file
</commit_message>
<xml_diff>
--- a/problem_file_suite/problem_files.xlsx
+++ b/problem_file_suite/problem_files.xlsx
@@ -1,43 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickit/Desktop/INT-Coursework-2021/problem_file_suite/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15638\Documents\vscode-workspace\INT-Coursework-2021\problem_file_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163821C8-CF9C-0C46-B8EC-08BAEA80B32A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0947A846-AC5F-4D82-AD2B-A31F37120863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="3340" windowWidth="18340" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$G$2:$G$17</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$2:$H$17</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$G$2:$G$17</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$H$2:$H$17</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -47,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,12 +58,20 @@
     <t>Area</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Planner's cost with 10 pliers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alerady equipped with 10 pliers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,13 +86,34 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,14 +125,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="适中" xfId="1" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -399,20 +416,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="5" max="6" width="18.5" customWidth="1"/>
+    <col min="5" max="6" width="18.453125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +451,11 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -458,8 +478,11 @@
       <c r="H2">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -482,8 +505,11 @@
       <c r="H3">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -503,11 +529,17 @@
       <c r="G4">
         <v>25</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -530,8 +562,11 @@
       <c r="H5">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -554,8 +589,11 @@
       <c r="H6">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -578,8 +616,11 @@
       <c r="H7">
         <v>126</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -602,8 +643,11 @@
       <c r="H8">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -626,8 +670,11 @@
       <c r="H9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -650,8 +697,11 @@
       <c r="H10">
         <v>201</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -674,8 +724,11 @@
       <c r="H11">
         <v>225</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -698,8 +751,11 @@
       <c r="H12">
         <v>263</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -722,8 +778,11 @@
       <c r="H13">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -746,8 +805,11 @@
       <c r="H14">
         <v>-1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -770,8 +832,11 @@
       <c r="H15">
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -794,8 +859,11 @@
       <c r="H16">
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
@@ -816,11 +884,15 @@
         <v>429</v>
       </c>
       <c r="H17">
+        <v>429</v>
+      </c>
+      <c r="I17">
         <v>429</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>